<commit_message>
Aggiunto scenario di test
</commit_message>
<xml_diff>
--- a/src/main/resources/test/each_template.xlsx
+++ b/src/main/resources/test/each_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Workspace\ExcelFromXMLObject\src\main\resources\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52AF6AB5-CB91-416B-A6FB-1F5FFB55F305}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99326AD1-A4D3-43BD-BE89-01E2ED461E06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="28800" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,12 +69,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="A13" authorId="0" shapeId="0" xr:uid="{E1C53C34-3338-4786-87C8-7782A20C7178}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jx:each(lastCell="H15", items="sub", var="ur", direction="DOWN")</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="9">
   <si>
     <t>Each Demo</t>
   </si>
@@ -89,13 +102,25 @@
   </si>
   <si>
     <t>*</t>
+  </si>
+  <si>
+    <t>${ur.getValueForColumnCode("STR001")}</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>${ur.getValueForColumnCode("STR007")}</t>
+  </si>
+  <si>
+    <t>****</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,8 +141,14 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,13 +157,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -158,12 +195,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,22 +482,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q11"/>
+  <dimension ref="A1:Q237"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="A238" sqref="A238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" s="3" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="2" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -472,26 +510,26 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="J6" s="4" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="J6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -553,6 +591,42 @@
       </c>
       <c r="M11" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="237" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>